<commit_message>
add in table defs
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E027565-0898-EC48-9542-5DD2180223C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B85872-7F01-5C45-8BF9-5E71D828171E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="crec_persons" sheetId="1" r:id="rId1"/>
-    <sheet name="crec_lookup" sheetId="2" r:id="rId2"/>
+    <sheet name="table_definitions" sheetId="3" r:id="rId1"/>
+    <sheet name="crec_persons" sheetId="1" r:id="rId2"/>
+    <sheet name="crec_lookup" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">crec_persons!$A$1:$P$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">crec_persons!$A$1:$P$82</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="128">
   <si>
     <t>table_name</t>
   </si>
@@ -460,12 +461,48 @@
   <si>
     <t>not mapped</t>
   </si>
+  <si>
+    <t>mapping_file_name</t>
+  </si>
+  <si>
+    <t>entity_name</t>
+  </si>
+  <si>
+    <t>required_entities</t>
+  </si>
+  <si>
+    <t>destination_table_name</t>
+  </si>
+  <si>
+    <t>table_type</t>
+  </si>
+  <si>
+    <t>source_table_name</t>
+  </si>
+  <si>
+    <t>casrec_conditions</t>
+  </si>
+  <si>
+    <t>source_table_additional_columns</t>
+  </si>
+  <si>
+    <t>crec_persons</t>
+  </si>
+  <si>
+    <t>crec</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -507,6 +544,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -576,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -609,6 +652,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,13 +868,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CC95F4-02E8-0A4B-AAFA-EC43C582E824}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
@@ -4113,7 +4219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4138,7 +4244,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
         <v>0</v>
       </c>
@@ -4150,7 +4256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -4162,7 +4268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -4174,7 +4280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
generate the complicated crec conditions order the table defs
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B85872-7F01-5C45-8BF9-5E71D828171E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CAA4B7-28F0-D044-9396-EAE7A0458E91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="129">
   <si>
     <t>table_name</t>
   </si>
@@ -496,6 +496,10 @@
   </si>
   <si>
     <t>data</t>
+  </si>
+  <si>
+    <t>convert_to_timestamp = {"date": "Modify", "time": "at.1"} 
+latest = {"col": "timestamp", "per": "Case"}</t>
   </si>
 </sst>
 </file>
@@ -619,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -650,10 +654,13 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -871,56 +878,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CC95F4-02E8-0A4B-AAFA-EC43C582E824}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="7" max="7" width="49.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:8" s="19" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A2" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="21" t="s">
+      <c r="D2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="19" t="s">
         <v>125</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2367,8 +2380,8 @@
       <c r="D50" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E50" s="18"/>
-      <c r="F50" s="19"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="21"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
@@ -2423,8 +2436,8 @@
       <c r="D52" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E52" s="18"/>
-      <c r="F52" s="19"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="21"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
@@ -3067,8 +3080,8 @@
       <c r="D75" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E75" s="18"/>
-      <c r="F75" s="19"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="21"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
@@ -3125,8 +3138,8 @@
       <c r="D77" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E77" s="18"/>
-      <c r="F77" s="19"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="21"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
@@ -3215,8 +3228,8 @@
       <c r="D80" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E80" s="18"/>
-      <c r="F80" s="19"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="21"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>

</xml_diff>

<commit_message>
missed the extra fields
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CAA4B7-28F0-D044-9396-EAE7A0458E91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF15AAD-9051-D244-AAF7-815DC5EFE8BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="130">
   <si>
     <t>table_name</t>
   </si>
@@ -500,6 +500,9 @@
   <si>
     <t>convert_to_timestamp = {"date": "Modify", "time": "at.1"} 
 latest = {"col": "timestamp", "per": "Case"}</t>
+  </si>
+  <si>
+    <t>Modify, at.1, Case</t>
   </si>
 </sst>
 </file>
@@ -656,11 +659,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,7 +882,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -932,8 +935,11 @@
       <c r="F2" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="20" t="s">
         <v>128</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2380,8 +2386,8 @@
       <c r="D50" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E50" s="20"/>
-      <c r="F50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="22"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
@@ -2436,8 +2442,8 @@
       <c r="D52" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E52" s="20"/>
-      <c r="F52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="22"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
@@ -3080,8 +3086,8 @@
       <c r="D75" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E75" s="20"/>
-      <c r="F75" s="21"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="22"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
@@ -3138,8 +3144,8 @@
       <c r="D77" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E77" s="20"/>
-      <c r="F77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="22"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
@@ -3228,8 +3234,8 @@
       <c r="D80" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E80" s="20"/>
-      <c r="F80" s="21"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="22"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>

</xml_diff>

<commit_message>
IN-957 Use "at" instead of "at.1" for crec
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B2E40A-55DB-F040-A3D6-7813E8B9AEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168F2FB4-92C1-D94F-A088-5444CBA8895C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21880" yWindow="4340" windowWidth="35840" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="3" r:id="rId1"/>
@@ -479,11 +479,11 @@
     <t>data</t>
   </si>
   <si>
-    <t>convert_to_timestamp = {"date": "Modify", "time": "at.1"} 
+    <t>Modify, at1, Case</t>
+  </si>
+  <si>
+    <t>convert_to_timestamp = {"date": "Modify", "time": "at1"} 
 latest = {"col": "timestamp", "per": "Case"}</t>
-  </si>
-  <si>
-    <t>Modify, at.1, Case</t>
   </si>
 </sst>
 </file>
@@ -842,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CC95F4-02E8-0A4B-AAFA-EC43C582E824}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -897,10 +897,10 @@
         <v>119</v>
       </c>
       <c r="G2" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>122</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -915,8 +915,8 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K79" sqref="K79"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
IN-940 Add mappings for fee reductions; Fix a small bug in Crec mapping
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC07027-D862-994D-906A-80371D58D9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D977B1F0-BA1D-3B45-86AE-7EE99BE72EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,9 +473,6 @@
     <t>crec</t>
   </si>
   <si>
-    <t>client</t>
-  </si>
-  <si>
     <t>data</t>
   </si>
   <si>
@@ -484,6 +481,9 @@
   <si>
     <t>convert_to_timestamp = {"date": "Modify", "time": "at"} 
 latest = {"col": "timestamp", "per": "Case"}</t>
+  </si>
+  <si>
+    <t>clients</t>
   </si>
 </sst>
 </file>
@@ -843,7 +843,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -885,22 +885,22 @@
         <v>119</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>120</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>121</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>119</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>